<commit_message>
Update HkmcVehicleInput/Output's Signal Matrixs for R2
</commit_message>
<xml_diff>
--- a/R2/02_SignalMatrix/HkmcVehOutputAdap/VehOutputAdap_SignalMatrix_V1_R2.xlsx
+++ b/R2/02_SignalMatrix/HkmcVehOutputAdap/VehOutputAdap_SignalMatrix_V1_R2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23007"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anjali.dayanand\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soo-jin.ahn\Veoneer\KHT HKMC BN7 FCA Project - SOS and MVS4\01_Engineering\03_SW and FD\ApplicationSoftware\FeatureSignalMatrixs\HkmcVehOutputAdap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{94AE4442-549D-4C6D-B512-25A02A5EDEDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{33A3128D-F47D-4B60-8652-1CBB250B0A0F}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="6_{A67D0E13-540E-41C4-9E61-34751E826F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D6AA43A-B2CC-465C-9D3B-187D0EC11BA3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="22" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="_ASIL_level_data">#REF!</definedName>
     <definedName name="_Comment">#REF!</definedName>
     <definedName name="_Comment_data">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Signals Detailed Information'!$A$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Signals Detailed Information'!$C$1:$C$92</definedName>
     <definedName name="_Implemented">#REF!</definedName>
     <definedName name="_Implemented_data">#REF!</definedName>
     <definedName name="_SWC_Allocation">#REF!</definedName>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="204">
   <si>
     <t>Change Log</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>HFA_OUTPUTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FcaAdap_WrngLvlSta </t>
   </si>
   <si>
     <t>enum</t>
@@ -195,9 +192,6 @@
 Cx2_PrefillAR_Reserved
 Cx3_PrefillAR_Error_Indicator</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">FcaAdap_DclReqVal </t>
   </si>
   <si>
     <t>uint8</t>
@@ -500,7 +494,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -510,7 +504,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -649,7 +643,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -659,7 +653,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -713,6 +707,9 @@
     <t>Cx0_LHW_No_Warning
 Cx1_LHW_HAPTIC_Warning_and_Display
 Cx2_LHW_Acoustic_Warning_and_Display</t>
+  </si>
+  <si>
+    <t>CF_LKA_RHWarning</t>
   </si>
   <si>
     <t>CF_LKA_SysWarning</t>
@@ -1042,26 +1039,66 @@
   <si>
     <t>HkmcVehicleOutputAdap</t>
   </si>
+  <si>
+    <t>HFA_OUTPUTS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HVOA_FCA11_FS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FCA_WrngSndSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">FcaAdap_DclReqVal </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HbaAdap_errorState</t>
+  </si>
+  <si>
+    <t>Cx0_ErS_HBA_activated
+Cx1_ErS_HBA_faulty
+Cx2_ErS_HBA_temporarily_not_available</t>
+  </si>
+  <si>
+    <t>HbaAdap_highBeamStateRequest</t>
+  </si>
+  <si>
+    <t>Cx0_HighBSR_Off
+Cx1_HighBSR_On
+Cx2_HighBSR_Partial_highbeam_on</t>
+  </si>
+  <si>
+    <t>enum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FcaAdap_WrngLvlSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1072,7 +1109,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1081,7 +1118,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1089,20 +1126,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1110,7 +1147,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1118,7 +1155,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1126,28 +1163,28 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1433,7 +1470,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -1452,9 +1489,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1569,7 +1603,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1617,6 +1651,22 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1624,6 +1674,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1684,7 +1743,7 @@
     <cellStyle name="Normal 8" xfId="12" xr:uid="{6299AA32-8A9F-43A0-9B69-D10D8C0FA74E}"/>
     <cellStyle name="Normal 9" xfId="14" xr:uid="{34EE8980-3288-4367-90A1-5B8B5546E1FF}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -1728,6 +1787,40 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
@@ -2077,17 +2170,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.75" thickBot="1">
+    <row r="1" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2120,15 +2213,15 @@
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="71"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2155,21 +2248,21 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="60"/>
+      <c r="F3" s="59"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2196,21 +2289,21 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="61">
+      <c r="B4" s="60">
         <v>1</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="52">
         <v>43990</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="61" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2"/>
@@ -2239,13 +2332,13 @@
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="64"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="63"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2272,13 +2365,13 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="62"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2305,13 +2398,13 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="64"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="63"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2338,13 +2431,13 @@
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="62"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -2371,13 +2464,13 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="64"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="63"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2404,13 +2497,13 @@
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="62"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="61"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2437,13 +2530,13 @@
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="63"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2470,13 +2563,13 @@
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="62"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="61"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2503,13 +2596,13 @@
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="63"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2536,13 +2629,13 @@
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="62"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="61"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2569,13 +2662,13 @@
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
     </row>
-    <row r="15" spans="1:31" ht="15.75" thickBot="1">
+    <row r="15" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="68"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="67"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2602,7 +2695,7 @@
       <c r="AD15" s="2"/>
       <c r="AE15" s="2"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2635,7 +2728,7 @@
       <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2668,7 +2761,7 @@
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2701,7 +2794,7 @@
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2734,7 +2827,7 @@
       <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2767,7 +2860,7 @@
       <c r="AD20" s="2"/>
       <c r="AE20" s="2"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2800,7 +2893,7 @@
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2833,7 +2926,7 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2866,7 +2959,7 @@
       <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2899,7 +2992,7 @@
       <c r="AD24" s="2"/>
       <c r="AE24" s="2"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2932,7 +3025,7 @@
       <c r="AD25" s="2"/>
       <c r="AE25" s="2"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2965,7 +3058,7 @@
       <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2998,7 +3091,7 @@
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3031,7 +3124,7 @@
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3064,7 +3157,7 @@
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3097,7 +3190,7 @@
       <c r="AD30" s="2"/>
       <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3130,7 +3223,7 @@
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3163,7 +3256,7 @@
       <c r="AD32" s="2"/>
       <c r="AE32" s="2"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3196,7 +3289,7 @@
       <c r="AD33" s="2"/>
       <c r="AE33" s="2"/>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3229,7 +3322,7 @@
       <c r="AD34" s="2"/>
       <c r="AE34" s="2"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3262,7 +3355,7 @@
       <c r="AD35" s="2"/>
       <c r="AE35" s="2"/>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3295,7 +3388,7 @@
       <c r="AD36" s="2"/>
       <c r="AE36" s="2"/>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3328,7 +3421,7 @@
       <c r="AD37" s="2"/>
       <c r="AE37" s="2"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3361,7 +3454,7 @@
       <c r="AD38" s="2"/>
       <c r="AE38" s="2"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -3394,7 +3487,7 @@
       <c r="AD39" s="2"/>
       <c r="AE39" s="2"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3427,7 +3520,7 @@
       <c r="AD40" s="2"/>
       <c r="AE40" s="2"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3460,7 +3553,7 @@
       <c r="AD41" s="2"/>
       <c r="AE41" s="2"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3493,7 +3586,7 @@
       <c r="AD42" s="2"/>
       <c r="AE42" s="2"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3526,7 +3619,7 @@
       <c r="AD43" s="2"/>
       <c r="AE43" s="2"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3559,7 +3652,7 @@
       <c r="AD44" s="2"/>
       <c r="AE44" s="2"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3592,7 +3685,7 @@
       <c r="AD45" s="2"/>
       <c r="AE45" s="2"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3625,7 +3718,7 @@
       <c r="AD46" s="2"/>
       <c r="AE46" s="2"/>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3658,7 +3751,7 @@
       <c r="AD47" s="2"/>
       <c r="AE47" s="2"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3691,7 +3784,7 @@
       <c r="AD48" s="2"/>
       <c r="AE48" s="2"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3724,7 +3817,7 @@
       <c r="AD49" s="2"/>
       <c r="AE49" s="2"/>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3769,1783 +3862,1689 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D27E9A-821C-4719-949E-ADFE999540AB}">
-  <dimension ref="B1:H90"/>
+  <dimension ref="B1:H92"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="40.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="45.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="42" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="4.125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="40.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="10" customWidth="1"/>
+    <col min="7" max="7" width="45.625" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.75" style="41" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="20.25" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:7" ht="45">
-      <c r="B2" s="13" t="s">
+    <row r="1" spans="2:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="60">
-      <c r="B3" s="17">
+    <row r="3" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="77" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B4" s="16">
+        <v>2</v>
+      </c>
+      <c r="C4" s="78"/>
+      <c r="D4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B5" s="16">
+        <v>3</v>
+      </c>
+      <c r="C5" s="78"/>
+      <c r="D5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="16">
+        <v>4</v>
+      </c>
+      <c r="C6" s="78"/>
+      <c r="D6" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="46"/>
+    </row>
+    <row r="7" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B7" s="16">
+        <v>5</v>
+      </c>
+      <c r="C7" s="78"/>
+      <c r="D7" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B8" s="16">
+        <v>6</v>
+      </c>
+      <c r="C8" s="78"/>
+      <c r="D8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B9" s="16">
+        <v>7</v>
+      </c>
+      <c r="C9" s="78"/>
+      <c r="D9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B10" s="16">
+        <v>8</v>
+      </c>
+      <c r="C10" s="78"/>
+      <c r="D10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <v>9</v>
+      </c>
+      <c r="C11" s="78"/>
+      <c r="D11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="16">
+        <v>10</v>
+      </c>
+      <c r="C12" s="78"/>
+      <c r="D12" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="46"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="16">
+        <v>11</v>
+      </c>
+      <c r="C13" s="78"/>
+      <c r="D13" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="46"/>
+    </row>
+    <row r="14" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B14" s="16">
+        <v>12</v>
+      </c>
+      <c r="C14" s="78"/>
+      <c r="D14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="16">
+        <v>13</v>
+      </c>
+      <c r="C15" s="78"/>
+      <c r="D15" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="42"/>
+    </row>
+    <row r="16" spans="2:7" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="16">
         <v>14</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="23" t="s">
+      <c r="C16" s="78"/>
+      <c r="D16" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G16" s="43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="16">
+        <v>15</v>
+      </c>
+      <c r="C17" s="78"/>
+      <c r="D17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="47"/>
+    </row>
+    <row r="18" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B18" s="16">
+        <v>16</v>
+      </c>
+      <c r="C18" s="78"/>
+      <c r="D18" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="16">
         <v>17</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="C19" s="78"/>
+      <c r="D19" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="42"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="16">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" ht="60">
-      <c r="B4" s="17">
-        <v>2</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="23" t="s">
+      <c r="C20" s="78"/>
+      <c r="D20" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="42"/>
+    </row>
+    <row r="21" spans="2:8" ht="132" x14ac:dyDescent="0.3">
+      <c r="B21" s="16">
         <v>19</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="C21" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="46" t="s">
+      <c r="G21" s="42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B22" s="16">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="60">
-      <c r="B5" s="17">
-        <v>3</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="23" t="s">
+      <c r="C22" s="77"/>
+      <c r="D22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="48"/>
+    </row>
+    <row r="23" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B23" s="16">
         <v>21</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="C23" s="77"/>
+      <c r="D23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="46" t="s">
+      <c r="G23" s="44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B24" s="16">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="17">
-        <v>4</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="23" t="s">
+      <c r="C24" s="77"/>
+      <c r="D24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B25" s="16">
         <v>23</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="C25" s="77"/>
+      <c r="D25" s="70" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="72" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B26" s="16">
         <v>24</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="47"/>
-    </row>
-    <row r="7" spans="2:7" ht="60">
-      <c r="B7" s="17">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="23" t="s">
+      <c r="C26" s="77"/>
+      <c r="D26" s="70" t="s">
+        <v>200</v>
+      </c>
+      <c r="E26" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="73" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="132" x14ac:dyDescent="0.3">
+      <c r="B27" s="16">
         <v>25</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="C27" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="46" t="s">
+      <c r="G27" s="44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B28" s="16">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="120">
-      <c r="B8" s="17">
-        <v>6</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="23" t="s">
+      <c r="C28" s="71"/>
+      <c r="D28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B29" s="16">
         <v>27</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="C29" s="71"/>
+      <c r="D29" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="46" t="s">
+      <c r="G29" s="44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="16">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="60">
-      <c r="B9" s="17">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="23" t="s">
+      <c r="C30" s="71"/>
+      <c r="D30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="42"/>
+    </row>
+    <row r="31" spans="2:8" ht="99" x14ac:dyDescent="0.3">
+      <c r="B31" s="16">
         <v>29</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="C31" s="71"/>
+      <c r="D31" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="46" t="s">
+      <c r="G31" s="42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="99" x14ac:dyDescent="0.3">
+      <c r="B32" s="16">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="120">
-      <c r="B10" s="17">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="23" t="s">
+      <c r="C32" s="71"/>
+      <c r="D32" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="264" x14ac:dyDescent="0.3">
+      <c r="B33" s="16">
         <v>31</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="C33" s="71"/>
+      <c r="D33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="46" t="s">
+      <c r="G33" s="44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="132" x14ac:dyDescent="0.3">
+      <c r="B34" s="16">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="120">
-      <c r="B11" s="17">
-        <v>9</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="23" t="s">
+      <c r="C34" s="71"/>
+      <c r="D34" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B35" s="16">
         <v>33</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="C35" s="71"/>
+      <c r="D35" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="46" t="s">
+      <c r="G35" s="44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="B36" s="16">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="17">
-        <v>10</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="23" t="s">
+      <c r="C36" s="71"/>
+      <c r="D36" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="132" x14ac:dyDescent="0.3">
+      <c r="B37" s="16">
         <v>35</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="C37" s="71"/>
+      <c r="D37" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="16">
         <v>36</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="17">
-        <v>11</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="23" t="s">
+      <c r="C38" s="77" t="s">
+        <v>195</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G38" s="43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="16">
         <v>37</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="C39" s="78"/>
+      <c r="D39" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G39" s="43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="33" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="16">
         <v>38</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="47"/>
-    </row>
-    <row r="14" spans="2:7" ht="120">
-      <c r="B14" s="17">
-        <v>12</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="23" t="s">
+      <c r="C40" s="78"/>
+      <c r="D40" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" s="43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="16">
         <v>39</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="46" t="s">
+      <c r="C41" s="78"/>
+      <c r="D41" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" s="42"/>
+    </row>
+    <row r="42" spans="2:8" ht="33" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="16">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="17">
-        <v>13</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="23" t="s">
+      <c r="C42" s="78"/>
+      <c r="D42" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G42" s="43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="49.5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="16">
         <v>41</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="C43" s="78"/>
+      <c r="D43" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G43" s="43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="33" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="16">
         <v>42</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="43"/>
-    </row>
-    <row r="16" spans="2:7" ht="105">
-      <c r="B16" s="17">
-        <v>14</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="23" t="s">
+      <c r="C44" s="78"/>
+      <c r="D44" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G44" s="43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="16">
         <v>43</v>
       </c>
-      <c r="E16" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="44" t="s">
+      <c r="C45" s="78"/>
+      <c r="D45" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G45" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="H45" s="48"/>
+    </row>
+    <row r="46" spans="2:8" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="16">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="17">
-        <v>15</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="23" t="s">
+      <c r="C46" s="78"/>
+      <c r="D46" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G46" s="43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="16">
         <v>45</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="C47" s="78"/>
+      <c r="D47" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G47" s="42"/>
+    </row>
+    <row r="48" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="16">
         <v>46</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="48"/>
-    </row>
-    <row r="18" spans="2:8" ht="60">
-      <c r="B18" s="17">
-        <v>16</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="23" t="s">
+      <c r="C48" s="78"/>
+      <c r="D48" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G48" s="42"/>
+    </row>
+    <row r="49" spans="2:7" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="16">
         <v>47</v>
       </c>
-      <c r="E18" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="44" t="s">
+      <c r="C49" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="16">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="17">
-        <v>17</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="23" t="s">
+      <c r="C50" s="78"/>
+      <c r="D50" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G50" s="43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="16">
         <v>49</v>
       </c>
-      <c r="E19" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="43"/>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="17">
-        <v>18</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="23" t="s">
+      <c r="C51" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G51" s="42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="33" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="16">
         <v>50</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="C52" s="78"/>
+      <c r="D52" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" s="44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="33" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="16">
         <v>51</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="43"/>
-    </row>
-    <row r="21" spans="2:8" ht="120">
-      <c r="B21" s="17">
-        <v>19</v>
-      </c>
-      <c r="C21" s="10" t="s">
+      <c r="C53" s="78"/>
+      <c r="D53" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G53" s="44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="16">
         <v>52</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="C54" s="78"/>
+      <c r="D54" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="16">
         <v>53</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="43" t="s">
+      <c r="C55" s="78"/>
+      <c r="D55" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G55" s="44"/>
+    </row>
+    <row r="56" spans="2:7" ht="33" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="16">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="60">
-      <c r="B22" s="17">
-        <v>20</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="C56" s="78"/>
+      <c r="D56" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G56" s="42" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="33" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="16">
+        <v>55</v>
+      </c>
+      <c r="C57" s="78"/>
+      <c r="D57" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="16">
+        <v>56</v>
+      </c>
+      <c r="C58" s="78"/>
+      <c r="D58" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G58" s="42"/>
+    </row>
+    <row r="59" spans="2:7" ht="49.5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="16">
+        <v>57</v>
+      </c>
+      <c r="C59" s="78"/>
+      <c r="D59" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G59" s="42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="49.5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="16">
+        <v>58</v>
+      </c>
+      <c r="C60" s="78"/>
+      <c r="D60" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G60" s="42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="49.5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="16">
+        <v>59</v>
+      </c>
+      <c r="C61" s="78"/>
+      <c r="D61" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G61" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="16">
+        <v>60</v>
+      </c>
+      <c r="C62" s="78"/>
+      <c r="D62" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G62" s="44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="33" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="16">
+        <v>61</v>
+      </c>
+      <c r="C63" s="78"/>
+      <c r="D63" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G63" s="44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="16">
+        <v>62</v>
+      </c>
+      <c r="C64" s="78"/>
+      <c r="D64" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G64" s="44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="16">
+        <v>63</v>
+      </c>
+      <c r="C65" s="78"/>
+      <c r="D65" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G65" s="44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B66" s="16">
+        <v>64</v>
+      </c>
+      <c r="C66" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E66" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G66" s="43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B67" s="16">
+        <v>65</v>
+      </c>
+      <c r="C67" s="78"/>
+      <c r="D67" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G67" s="43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B68" s="16">
+        <v>66</v>
+      </c>
+      <c r="C68" s="78"/>
+      <c r="D68" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G68" s="43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69" s="16">
+        <v>67</v>
+      </c>
+      <c r="C69" s="78"/>
+      <c r="D69" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G69" s="42"/>
+    </row>
+    <row r="70" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B70" s="16">
+        <v>68</v>
+      </c>
+      <c r="C70" s="78"/>
+      <c r="D70" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G70" s="43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B71" s="16">
+        <v>69</v>
+      </c>
+      <c r="C71" s="78"/>
+      <c r="D71" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G71" s="43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B72" s="16">
+        <v>70</v>
+      </c>
+      <c r="C72" s="78"/>
+      <c r="D72" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G72" s="43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B73" s="16">
+        <v>71</v>
+      </c>
+      <c r="C73" s="78"/>
+      <c r="D73" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G73" s="43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B74" s="16">
+        <v>72</v>
+      </c>
+      <c r="C74" s="78"/>
+      <c r="D74" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G74" s="43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B75" s="16">
+        <v>73</v>
+      </c>
+      <c r="C75" s="78"/>
+      <c r="D75" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G75" s="42"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B76" s="16">
+        <v>74</v>
+      </c>
+      <c r="C76" s="78"/>
+      <c r="D76" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G76" s="42"/>
+    </row>
+    <row r="77" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B77" s="16">
+        <v>75</v>
+      </c>
+      <c r="C77" s="78"/>
+      <c r="D77" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E77" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G77" s="43" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B78" s="16">
+        <v>76</v>
+      </c>
+      <c r="C78" s="77" t="s">
+        <v>155</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G78" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="49"/>
-    </row>
-    <row r="23" spans="2:8" ht="60">
-      <c r="B23" s="17">
-        <v>21</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="60">
-      <c r="B24" s="17">
-        <v>22</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="120">
-      <c r="B25" s="17">
-        <v>23</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="45" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="60">
-      <c r="B26" s="17">
-        <v>24</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="60">
-      <c r="B27" s="17">
-        <v>25</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="45" t="s">
+    </row>
+    <row r="79" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B79" s="16">
+        <v>77</v>
+      </c>
+      <c r="C79" s="78"/>
+      <c r="D79" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G79" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B80" s="16">
+        <v>78</v>
+      </c>
+      <c r="C80" s="78"/>
+      <c r="D80" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G80" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B81" s="16">
+        <v>79</v>
+      </c>
+      <c r="C81" s="78"/>
+      <c r="D81" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G81" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B82" s="16">
+        <v>80</v>
+      </c>
+      <c r="C82" s="78" t="s">
+        <v>163</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G82" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B83" s="16">
+        <v>81</v>
+      </c>
+      <c r="C83" s="78"/>
+      <c r="D83" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G83" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B84" s="16">
+        <v>82</v>
+      </c>
+      <c r="C84" s="78"/>
+      <c r="D84" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G84" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B85" s="16">
+        <v>83</v>
+      </c>
+      <c r="C85" s="78"/>
+      <c r="D85" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E85" s="9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="B28" s="17">
-        <v>26</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="43"/>
-    </row>
-    <row r="29" spans="2:8" ht="90">
-      <c r="B29" s="17">
-        <v>27</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="90">
-      <c r="B30" s="17">
-        <v>28</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="43" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="240">
-      <c r="B31" s="17">
-        <v>29</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="45" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="120">
-      <c r="B32" s="17">
-        <v>30</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="45" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="60">
-      <c r="B33" s="17">
-        <v>31</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="45" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="60">
-      <c r="B34" s="17">
-        <v>32</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="120">
-      <c r="B35" s="17">
-        <v>33</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="60" outlineLevel="1">
-      <c r="B36" s="17">
-        <v>34</v>
-      </c>
-      <c r="C36" s="10" t="s">
+      <c r="F85" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="G85" s="18"/>
+    </row>
+    <row r="86" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B86" s="16">
+        <v>84</v>
+      </c>
+      <c r="C86" s="78"/>
+      <c r="D86" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G86" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B87" s="16">
         <v>85</v>
       </c>
-      <c r="E36" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="8" t="s">
+      <c r="C87" s="78"/>
+      <c r="D87" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G87" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" ht="264" x14ac:dyDescent="0.3">
+      <c r="B88" s="16">
         <v>86</v>
       </c>
-      <c r="G36" s="44" t="s">
+      <c r="C88" s="78"/>
+      <c r="D88" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G88" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B89" s="16">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" ht="60" outlineLevel="1">
-      <c r="B37" s="17">
-        <v>35</v>
-      </c>
-      <c r="C37" s="10" t="s">
+      <c r="C89" s="78"/>
+      <c r="D89" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F89" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="G89" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B90" s="16">
         <v>88</v>
       </c>
-      <c r="E37" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G37" s="44" t="s">
+      <c r="C90" s="78"/>
+      <c r="D90" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G90" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B91" s="16">
         <v>89</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" ht="30" outlineLevel="1">
-      <c r="B38" s="17">
-        <v>36</v>
-      </c>
-      <c r="C38" s="10" t="s">
+      <c r="C91" s="78"/>
+      <c r="D91" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F91" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="G91" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="132.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="19">
         <v>90</v>
       </c>
-      <c r="E38" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G38" s="44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" outlineLevel="1">
-      <c r="B39" s="17">
-        <v>37</v>
-      </c>
-      <c r="C39" s="10" t="s">
+      <c r="C92" s="79"/>
+      <c r="D92" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F92" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G39" s="43"/>
-    </row>
-    <row r="40" spans="2:8" ht="30" outlineLevel="1">
-      <c r="B40" s="17">
-        <v>38</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G40" s="44" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="45" outlineLevel="1">
-      <c r="B41" s="17">
-        <v>39</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G41" s="44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="30" outlineLevel="1">
-      <c r="B42" s="17">
-        <v>40</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="60" outlineLevel="1">
-      <c r="B43" s="17">
-        <v>41</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G43" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="H43" s="49"/>
-    </row>
-    <row r="44" spans="2:8" ht="120" outlineLevel="1">
-      <c r="B44" s="17">
-        <v>42</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G44" s="44" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" outlineLevel="1">
-      <c r="B45" s="17">
-        <v>43</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G45" s="43"/>
-    </row>
-    <row r="46" spans="2:8" outlineLevel="1">
-      <c r="B46" s="17">
-        <v>44</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G46" s="43"/>
-    </row>
-    <row r="47" spans="2:8" ht="120" outlineLevel="1">
-      <c r="B47" s="17">
-        <v>45</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G47" s="44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="120" outlineLevel="1">
-      <c r="B48" s="17">
-        <v>46</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G48" s="44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="60" outlineLevel="1">
-      <c r="B49" s="17">
-        <v>47</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G49" s="43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="30" outlineLevel="1">
-      <c r="B50" s="17">
-        <v>48</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G50" s="45" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" ht="30" outlineLevel="1">
-      <c r="B51" s="17">
-        <v>49</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G51" s="45" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" ht="60" outlineLevel="1">
-      <c r="B52" s="17">
-        <v>50</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G52" s="45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" outlineLevel="1">
-      <c r="B53" s="17">
-        <v>51</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G53" s="45"/>
-    </row>
-    <row r="54" spans="2:7" ht="30" outlineLevel="1">
-      <c r="B54" s="17">
-        <v>52</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G54" s="43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="30" outlineLevel="1">
-      <c r="B55" s="17">
-        <v>53</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G55" s="45" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" outlineLevel="1">
-      <c r="B56" s="17">
-        <v>54</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D56" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G56" s="43"/>
-    </row>
-    <row r="57" spans="2:7" ht="45" outlineLevel="1">
-      <c r="B57" s="17">
-        <v>55</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G57" s="43" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="45" outlineLevel="1">
-      <c r="B58" s="17">
-        <v>56</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G58" s="43" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="45" outlineLevel="1">
-      <c r="B59" s="17">
-        <v>57</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G59" s="45" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" ht="60" outlineLevel="1">
-      <c r="B60" s="17">
-        <v>58</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G60" s="45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="30" outlineLevel="1">
-      <c r="B61" s="17">
-        <v>59</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G61" s="45" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="60" outlineLevel="1">
-      <c r="B62" s="17">
-        <v>60</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G62" s="45" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" ht="120" outlineLevel="1">
-      <c r="B63" s="17">
-        <v>61</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G63" s="45" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" ht="60">
-      <c r="B64" s="17">
-        <v>62</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D64" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="E64" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G64" s="44" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" ht="60">
-      <c r="B65" s="17">
-        <v>63</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D65" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E65" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G65" s="44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" ht="60">
-      <c r="B66" s="17">
-        <v>64</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D66" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="E66" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G66" s="44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7">
-      <c r="B67" s="17">
-        <v>65</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D67" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="E67" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G67" s="43"/>
-    </row>
-    <row r="68" spans="2:7" ht="60">
-      <c r="B68" s="17">
-        <v>66</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D68" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E68" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G68" s="44" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" ht="120">
-      <c r="B69" s="17">
-        <v>67</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D69" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="E69" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G69" s="44" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" ht="60">
-      <c r="B70" s="17">
-        <v>68</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D70" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E70" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G70" s="44" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" ht="120">
-      <c r="B71" s="17">
-        <v>69</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D71" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="E71" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G71" s="44" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" ht="120">
-      <c r="B72" s="17">
-        <v>70</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D72" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="E72" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G72" s="44" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7">
-      <c r="B73" s="17">
-        <v>71</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D73" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="E73" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G73" s="43"/>
-    </row>
-    <row r="74" spans="2:7">
-      <c r="B74" s="17">
-        <v>72</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D74" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="E74" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G74" s="43"/>
-    </row>
-    <row r="75" spans="2:7" ht="120">
-      <c r="B75" s="17">
-        <v>73</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D75" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="E75" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F75" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G75" s="44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" ht="120">
-      <c r="B76" s="17">
-        <v>74</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G76" s="43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" ht="60">
-      <c r="B77" s="17">
-        <v>75</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G77" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" ht="60">
-      <c r="B78" s="17">
-        <v>76</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G78" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" ht="60">
-      <c r="B79" s="17">
-        <v>77</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G79" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" ht="120">
-      <c r="B80" s="17">
-        <v>78</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F80" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G80" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" ht="60">
-      <c r="B81" s="17">
-        <v>79</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G81" s="19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" ht="60">
-      <c r="B82" s="17">
-        <v>80</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G82" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7">
-      <c r="B83" s="17">
-        <v>81</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G83" s="19"/>
-    </row>
-    <row r="84" spans="2:7" ht="60">
-      <c r="B84" s="17">
-        <v>82</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G84" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" ht="60">
-      <c r="B85" s="17">
-        <v>83</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G85" s="19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" ht="240">
-      <c r="B86" s="17">
-        <v>84</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G86" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" ht="120">
-      <c r="B87" s="17">
-        <v>85</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F87" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G87" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" ht="60">
-      <c r="B88" s="17">
-        <v>86</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F88" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G88" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" ht="60">
-      <c r="B89" s="17">
-        <v>87</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G89" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" ht="120.75" thickBot="1">
-      <c r="B90" s="20">
-        <v>88</v>
-      </c>
-      <c r="C90" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="D90" s="21" t="s">
+      <c r="G92" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="E90" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F90" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G90" s="50" t="s">
-        <v>185</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C3:C20"/>
+    <mergeCell ref="C66:C77"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C92"/>
+    <mergeCell ref="C38:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C65"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="F3:F90">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+  <conditionalFormatting sqref="F3:F24 F27:F92">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Output"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"Input"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:F26">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"Output"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>"Input"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:F26">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"Output"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Input"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F90" xr:uid="{7D10BEF8-E409-4D08-84CA-2E9809A6BA79}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F92" xr:uid="{7D10BEF8-E409-4D08-84CA-2E9809A6BA79}">
       <formula1>"Input,Output"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5560,167 +5559,167 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.875" customWidth="1"/>
+    <col min="3" max="3" width="35.75" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.75" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10">
-      <c r="B2" s="72" t="s">
+    <row r="1" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="81"/>
+      <c r="D2" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="78" t="s">
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="87"/>
+    </row>
+    <row r="3" spans="2:10" s="28" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="79"/>
-    </row>
-    <row r="3" spans="2:10" s="29" customFormat="1" ht="58.5" customHeight="1">
-      <c r="B3" s="74"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="C4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="16.5" customHeight="1">
-      <c r="B4" s="76" t="s">
+      <c r="E4" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="30"/>
+      <c r="H4" s="29"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="33"/>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="76"/>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="84"/>
       <c r="C5" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="76"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="84"/>
       <c r="C6" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="34"/>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="76"/>
+        <v>189</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="33"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="84"/>
       <c r="C7" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="30"/>
+        <v>84</v>
+      </c>
+      <c r="E7" s="29"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="31"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="35"/>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="76"/>
+      <c r="J7" s="34"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="84"/>
       <c r="C8" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="J8" s="35"/>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B9" s="77"/>
-      <c r="C9" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="40" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="25"/>
+        <v>189</v>
+      </c>
+      <c r="J8" s="34"/>
+    </row>
+    <row r="9" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="85"/>
+      <c r="C9" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="39" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5753,88 +5752,88 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:7">
-      <c r="B2" s="72" t="s">
+    <row r="1" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="80" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="81"/>
+      <c r="D2" s="90" t="s">
         <v>191</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="82" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="84"/>
-    </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="74"/>
-      <c r="C3" s="75"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="92"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="84" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B4" s="76" t="s">
-        <v>194</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F4" s="7"/>
-      <c r="G4" s="35"/>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="80"/>
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="88"/>
       <c r="C5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G5" s="35"/>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B6" s="81"/>
-      <c r="C6" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="89"/>
+      <c r="C6" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="39" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -6099,13 +6098,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137238F2-A448-486B-B5AE-DB4CAF4A8984}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137238F2-A448-486B-B5AE-DB4CAF4A8984}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
+    <ds:schemaRef ds:uri="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>